<commit_message>
Fehler behoben initSpielfeld, zaehlLebende verinfacht
</commit_message>
<xml_diff>
--- a/Zeiten.xlsx
+++ b/Zeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\janes\Kompelieren\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A7E3AF-3C77-4AC6-988F-CABF44E0815E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977EB73B-FAE9-4D61-BDDA-60432191A9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Anfangs Code</t>
+  </si>
+  <si>
+    <t>Variablen Char</t>
+  </si>
+  <si>
+    <t>Janes</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>array =&gt; spielfeld</t>
+  </si>
+  <si>
+    <t>zaehleLebende vereinfacht</t>
   </si>
 </sst>
 </file>
@@ -345,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C3"/>
+  <dimension ref="A3:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -357,12 +372,48 @@
     <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
         <v>56.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
findNachbarn und zaehle beide zusammengefasst in einem Code und Methoden Aufruf entfernt
</commit_message>
<xml_diff>
--- a/Zeiten.xlsx
+++ b/Zeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\janes\Kompelieren\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9DB8E-3515-4646-BE92-06DE955E9A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86C200D-2132-470A-94B9-C0C66FBA4F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Anfangs Code</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>pruefeRegeln vereinfacht</t>
+  </si>
+  <si>
+    <t>printSpielfeld vereinfacht</t>
+  </si>
+  <si>
+    <t>Compiler Optimierung cmd</t>
+  </si>
+  <si>
+    <t>findNachbarn u. zaehleLebnde zusammengefasst u. Methoden Aufruf entfernt</t>
+  </si>
+  <si>
+    <t>pruefeRegeln vereinfacht u. Methoden Aufruf entfernt</t>
   </si>
 </sst>
 </file>
@@ -363,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C7"/>
+  <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="65.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -430,6 +442,50 @@
         <v>24.3</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>7.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Variable spielfeld u. temp geändert auf char
</commit_message>
<xml_diff>
--- a/Zeiten.xlsx
+++ b/Zeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\janes\Kompelieren\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86C200D-2132-470A-94B9-C0C66FBA4F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE7646C-8F88-42B2-80D6-0855A12FBE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Anfangs Code</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>pruefeRegeln vereinfacht u. Methoden Aufruf entfernt</t>
+  </si>
+  <si>
+    <t>printSpielfeld Methoden Aufruf entfernt</t>
+  </si>
+  <si>
+    <t>Variable spielfeld u. temp =&gt; char</t>
   </si>
 </sst>
 </file>
@@ -110,6 +116,917 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$3:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Anfangs Code</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Variablen Char</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>array =&gt; spielfeld</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>zaehleLebende vereinfacht</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pruefeRegeln vereinfacht</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>printSpielfeld vereinfacht</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pruefeRegeln vereinfacht u. Methoden Aufruf entfernt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Compiler Optimierung cmd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>findNachbarn u. zaehleLebnde zusammengefasst u. Methoden Aufruf entfernt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>56.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52F6-4037-9007-DA7A0E7B0CA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2075061855"/>
+        <c:axId val="2075051775"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2075061855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2075051775"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2075051775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2075061855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28A810D-3B5F-381C-89FA-7B97F986E509}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C11"/>
+  <dimension ref="A3:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +1403,30 @@
         <v>7.7</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>